<commit_message>
update function read file import
</commit_message>
<xml_diff>
--- a/document/Design/SignOutSystem.xlsx
+++ b/document/Design/SignOutSystem.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev_Project\Source_BookSaleReactJs\document\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\v_5\Source_BookSaleReactJs\document\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E14606-5A74-4CB8-A7CC-67F1B65F01C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +24,16 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Mô tả chức năng SignOut Sytem</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,6 +80,217 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF1F144C-2537-040F-1C13-44F9A34685C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="762000"/>
+          <a:ext cx="1228725" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Input</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Data</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59AC279D-0612-034E-0B58-ADAC231C48A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1828800" y="1333500"/>
+          <a:ext cx="4763" cy="10563225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle: Rounded Corners 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3A8FCBC-6E26-F358-F25F-45E245419C66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="2286001"/>
+          <a:ext cx="1866900" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Lấy</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Token và Local  Stored</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -335,14 +555,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>